<commit_message>
Updated package from Gareth
</commit_message>
<xml_diff>
--- a/Integration Services Project2/notes/NEL1902_SSIS_PKG Script_Conversion_Status.xlsx
+++ b/Integration Services Project2/notes/NEL1902_SSIS_PKG Script_Conversion_Status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\STE.2022.CoswinMigration\Integration Services Project2\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4068C7E-C642-41E7-B16E-1A036A783E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70CCA485-EF49-4BD0-AD33-8DAF9E773D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="539">
   <si>
     <t>SSIS Package Name</t>
   </si>
@@ -1808,16 +1808,10 @@
 WIP_WA</t>
   </si>
   <si>
-    <t>WOACTIVITY</t>
-  </si>
-  <si>
     <t>LABTRANS</t>
   </si>
   <si>
     <t>WIP_WE</t>
-  </si>
-  <si>
-    <t>SR</t>
   </si>
   <si>
     <t>EQP_JOBR</t>
@@ -1864,6 +1858,9 @@
   <si>
     <t>Why DF for INVOICE_ is disabled?
 Can we use SQL for INVOICECOST?</t>
+  </si>
+  <si>
+    <t>TICKET</t>
   </si>
 </sst>
 </file>
@@ -8390,7 +8387,7 @@
         <v>429</v>
       </c>
       <c r="C4" s="87" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="D4" s="81" t="s">
         <v>443</v>
@@ -10437,7 +10434,7 @@
   <dimension ref="A1:G178"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10981,10 +10978,10 @@
         <v>314</v>
       </c>
       <c r="C43" s="86" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="E43" s="83" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="F43" s="85" t="s">
         <v>509</v>
@@ -11032,10 +11029,10 @@
         <v>314</v>
       </c>
       <c r="C46" s="86" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="E46" s="83" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="F46" s="83" t="s">
         <v>515</v>
@@ -11058,7 +11055,7 @@
         <v>516</v>
       </c>
       <c r="G47" s="70" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -11126,7 +11123,7 @@
         <v>474</v>
       </c>
       <c r="E51" s="14" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="F51" s="14" t="s">
         <v>523</v>
@@ -11146,10 +11143,10 @@
         <v>474</v>
       </c>
       <c r="E52" s="14" t="s">
+        <v>525</v>
+      </c>
+      <c r="F52" s="84" t="s">
         <v>526</v>
-      </c>
-      <c r="F52" s="84" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -11163,10 +11160,10 @@
         <v>468</v>
       </c>
       <c r="E53" s="14" t="s">
-        <v>528</v>
+        <v>538</v>
       </c>
       <c r="F53" s="84" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -11180,7 +11177,7 @@
         <v>468</v>
       </c>
       <c r="E54" s="14" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="F54" s="84" t="s">
         <v>463</v>
@@ -11200,10 +11197,10 @@
         <v>475</v>
       </c>
       <c r="E55" s="14" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="F55" s="83" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -11220,7 +11217,7 @@
         <v>513</v>
       </c>
       <c r="F56" s="85" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>